<commit_message>
Updated BOM buttons and re-arranged lib folders
</commit_message>
<xml_diff>
--- a/MurrayTools.tab/Utilities.panel/ProjectUtilities.Stack/Exports.pulldown/GenerateBulkBOM.pushbutton/MR-BOM.xlsx
+++ b/MurrayTools.tab/Utilities.panel/ProjectUtilities.Stack/Exports.pulldown/GenerateBulkBOM.pushbutton/MR-BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Egnyte\Shared\BIM\Murray CADetailing Dept\REVIT\MURRAY RIBBON\Murray.extension\MurrayTools.tab\Utilities.panel\ProjectUtilities.Stack\Exports.pulldown\OpenBOMTemplate.pushbutton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Egnyte\Shared\BIM\Murray CADetailing Dept\REVIT\MURRAY RIBBON\Murray.extension\MurrayTools.tab\Utilities.panel\ProjectUtilities.Stack\Exports.pulldown\GenerateBulkBOM.pushbutton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910BA114-4FAA-47B5-9A87-030B37149B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EBBDAE-6ABC-4DCA-AB5B-756640DB97BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{3AEB8DE0-985F-4A48-8335-FFD4EE2C061B}"/>
+    <workbookView xWindow="-38520" yWindow="-1935" windowWidth="38640" windowHeight="21120" xr2:uid="{3AEB8DE0-985F-4A48-8335-FFD4EE2C061B}"/>
   </bookViews>
   <sheets>
     <sheet name="MEP Fabrication Pipe BOM" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
-        <charset val="204"/>
+        <family val="1"/>
       </rPr>
       <t>:</t>
     </r>
@@ -393,9 +393,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;\-0;;@"/>
-    <numFmt numFmtId="165" formatCode="0.00000_);\(0.00000\)"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -409,7 +408,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="204"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -660,6 +659,54 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -699,12 +746,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -714,53 +755,11 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1164,180 +1163,180 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="19"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="20"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="36"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="39"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="28" t="s">
+      <c r="A5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="25"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="28" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="40">
         <f ca="1">NOW()</f>
-        <v>45771.420253009259</v>
-      </c>
-      <c r="G7" s="27"/>
+        <v>45775.321327662037</v>
+      </c>
+      <c r="G7" s="41"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="31"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="44"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="31"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
       <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="25"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="31"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
       <c r="E11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="25"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="36"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="41"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="44"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="31"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="38"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
@@ -1367,22 +1366,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="F10:G10"/>
     <mergeCell ref="A1:D7"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="E2:G2"/>
@@ -1391,6 +1374,22 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>